<commit_message>
Worth agency name correction.
Fixed formatting of agency_number so that Park Forest joins correctly.
</commit_message>
<xml_diff>
--- a/Necessary_Files/muni_shortnames.xlsx
+++ b/Necessary_Files/muni_shortnames.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\OneDrive\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\ptax\Necessary_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D53708-1436-4F7E-B64C-928AC62231D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAED0BA-BB7C-4A65-92F7-BBBF09A3F27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="9030" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="4" xr2:uid="{E04B2839-4174-4D46-99FA-03AE29BCB57B}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{E04B2839-4174-4D46-99FA-03AE29BCB57B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1864,7 +1864,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1916,11 +1916,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1937,12 +1946,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="36">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -2310,7 +2320,13 @@
       </fill>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
@@ -2319,12 +2335,16 @@
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
@@ -2333,12 +2353,16 @@
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
@@ -2347,12 +2371,16 @@
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
@@ -2361,12 +2389,16 @@
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="thin">
@@ -2375,8 +2407,43 @@
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2385,6 +2452,14 @@
           <color theme="4" tint="0.39997558519241921"/>
         </left>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -5696,17 +5771,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D179A9D4-42CB-495B-8B63-9C6B4EB0A0D5}" name="Table1" displayName="Table1" ref="A1:E135" totalsRowShown="0" headerRowDxfId="32" tableBorderDxfId="31">
-  <autoFilter ref="A1:E135" xr:uid="{D179A9D4-42CB-495B-8B63-9C6B4EB0A0D5}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E135">
-    <sortCondition ref="A1:A135"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D179A9D4-42CB-495B-8B63-9C6B4EB0A0D5}" name="Table1" displayName="Table1" ref="A1:G135" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
+  <autoFilter ref="A1:G135" xr:uid="{D179A9D4-42CB-495B-8B63-9C6B4EB0A0D5}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F135">
+    <sortCondition ref="B1:B135"/>
   </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1F9C6787-AF3E-42F8-88E4-235AC1C1596A}" name="agency_number" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{6683F83A-27AA-4C73-8EA3-37CB28F7EE6C}" name="agency_name" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{8CA706FA-B778-4359-AA83-9B733DBD6530}" name="clean_name" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{CE881981-CE3C-4963-98DD-50D452D4C1BA}" name="Triad" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{0D872AF7-A538-48C8-BDC8-6BFDCB709A1B}" name="Township" dataDxfId="26"/>
+  <tableColumns count="7">
+    <tableColumn id="3" xr3:uid="{3C54D679-719C-4642-8295-74E3C545D08C}" name="short_name" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{1F9C6787-AF3E-42F8-88E4-235AC1C1596A}" name="agency_number" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{6683F83A-27AA-4C73-8EA3-37CB28F7EE6C}" name="agency_name" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{8CA706FA-B778-4359-AA83-9B733DBD6530}" name="clean_name" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{CE881981-CE3C-4963-98DD-50D452D4C1BA}" name="Triad" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{0D872AF7-A538-48C8-BDC8-6BFDCB709A1B}" name="Township" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{E3D2D05E-B6DC-41A0-94A4-1D6D02A852E5}" name="shpfile_name" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6094,3118 +6171,3119 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78B4136-5499-4584-8CDE-B5921A95B643}">
   <dimension ref="A1:G135"/>
   <sheetViews>
-    <sheetView zoomScale="63" workbookViewId="0">
-      <selection activeCell="F134" sqref="F134"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="63" workbookViewId="0">
+      <selection activeCell="G135" sqref="G135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.1" x14ac:dyDescent="0.8"/>
   <cols>
-    <col min="1" max="1" width="14.9296875" customWidth="1"/>
-    <col min="2" max="2" width="12.9296875" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="5" max="5" width="13.09765625" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.9296875" customWidth="1"/>
+    <col min="3" max="3" width="22.19921875" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.8">
       <c r="A1" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>406</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A2" s="3">
+      <c r="A2" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="B2" s="5">
         <v>20060000</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="15" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A3" s="5">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
         <v>30010000</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E3" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A4" s="3">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
         <v>30020000</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="5" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A5" s="5">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5">
         <v>30030000</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>295</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>5</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A6" s="3">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5">
         <v>30040000</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="5" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A7" s="5">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5">
         <v>30050000</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>420</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A8" s="3">
+      <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="5">
         <v>30060000</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="5" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A9" s="5">
+      <c r="A9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="5">
         <v>30070000</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E9" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>413</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A10" s="3">
+      <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="5">
         <v>30080000</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="5" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A11" s="5">
+      <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="5">
         <v>30090000</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E11" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>413</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A12" s="3">
+      <c r="A12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="5">
         <v>30100000</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="5" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A13" s="5">
+      <c r="A13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5">
         <v>30110000</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E13" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>417</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A14" s="3">
+      <c r="A14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="5">
         <v>30120000</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="5" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A15" s="5">
+      <c r="A15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="5">
         <v>30130000</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E15" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>413</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A16" s="3">
+      <c r="A16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="5">
         <v>30140000</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="5" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A17" s="5">
+      <c r="A17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="5">
         <v>30150000</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>394</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A18" s="3">
+      <c r="A18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="5">
         <v>30160000</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="5" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A19" s="3">
+      <c r="A19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="5">
         <v>30170000</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="5" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A20" s="5">
+      <c r="A20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="5">
         <v>30180000</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E20" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>346</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A21" s="5">
+      <c r="A21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="5">
         <v>30190000</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E21" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>389</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A22" s="3">
+      <c r="A22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="5">
         <v>30200000</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>417</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="5" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A23" s="3">
+      <c r="A23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="5">
         <v>30210000</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="5" t="s">
         <v>416</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="F23" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="5" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A24" s="5">
+      <c r="A24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="5">
         <v>30220000</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="D24" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E24" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>418</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A25" s="5">
+      <c r="A25" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="5">
         <v>30230000</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E25" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A26" s="3">
+      <c r="A26" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="5">
         <v>30240000</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="5" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A27" s="5">
+      <c r="A27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="5">
         <v>30250000</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E27" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>346</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A28" s="3">
+      <c r="A28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="5">
         <v>30260000</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="5" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A29" s="5">
+      <c r="A29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="5">
         <v>30270000</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>365</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A30" s="3">
+      <c r="A30" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="5">
         <v>30280000</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="F30" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="5" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A31" s="3">
+      <c r="A31" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="5">
         <v>30290000</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E31" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="F31" s="5" t="s">
         <v>411</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="5" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A32" s="5">
+      <c r="A32" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="5">
         <v>30300000</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="D32" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E32" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>389</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A33" s="3">
+      <c r="A33" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="5">
         <v>30310000</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="C33" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G33" s="3" t="s">
+      <c r="G33" s="5" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A34" s="5">
+      <c r="A34" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="5">
         <v>30320000</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="E34" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="F34" s="5" t="s">
         <v>295</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A35" s="3">
+      <c r="A35" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="5">
         <v>30330000</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="C35" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D35" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="5" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A36" s="5">
+      <c r="A36" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="5">
         <v>30340000</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="C36" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="D36" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="E36" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="F36" s="5" t="s">
         <v>420</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A37" s="5">
+      <c r="A37" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B37" s="5">
         <v>30350000</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="C37" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="D37" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="E37" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="F37" s="5" t="s">
         <v>424</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>270</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A38" s="3">
+      <c r="A38" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="5">
         <v>30370000</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="D38" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="E38" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="F38" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="F38" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G38" s="3" t="s">
+      <c r="G38" s="5" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A39" s="3">
+      <c r="A39" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="5">
         <v>30380000</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="C39" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="D39" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="E39" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="F39" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G39" s="3" t="s">
+      <c r="G39" s="5" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A40" s="5">
+      <c r="A40" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="5">
         <v>30390000</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="D40" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E40" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F40" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A41" s="3">
+      <c r="A41" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="5">
         <v>30400000</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="C41" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F41" s="5" t="s">
         <v>414</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G41" s="3" t="s">
+      <c r="G41" s="5" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A42" s="5">
+      <c r="A42" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="5">
         <v>30410000</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="C42" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="D42" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E42" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F42" s="5" t="s">
         <v>418</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A43" s="3">
+      <c r="A43" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="5">
         <v>30420000</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="C43" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G43" s="3" t="s">
+      <c r="G43" s="5" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A44" s="5">
+      <c r="A44" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="5">
         <v>30430000</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="C44" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="D44" s="5" t="s">
         <v>430</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E44" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F44" s="5" t="s">
         <v>385</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A45" s="3">
+      <c r="A45" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="5">
         <v>30440000</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="C45" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="D45" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F45" s="5" t="s">
         <v>414</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G45" s="3" t="s">
+      <c r="G45" s="5" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A46" s="5">
+      <c r="A46" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="5">
         <v>30450000</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="C46" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="D46" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="E46" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="F46" s="5" t="s">
         <v>419</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A47" s="3">
+      <c r="A47" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="5">
         <v>30460000</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="C47" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="D47" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="E47" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="F47" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="F47" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G47" s="3" t="s">
+      <c r="G47" s="5" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A48" s="5">
+      <c r="A48" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="5">
         <v>30470000</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="C48" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="D48" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="E48" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="F48" s="5" t="s">
         <v>358</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A49" s="3">
+      <c r="A49" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="5">
         <v>30480000</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="C49" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="D49" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E49" s="3" t="s">
+      <c r="E49" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F49" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="F49" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="G49" s="3" t="s">
+      <c r="G49" s="5" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A50" s="5">
+      <c r="A50" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" s="5">
         <v>30490000</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="C50" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="D50" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="E50" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="F50" s="5" t="s">
         <v>354</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A51" s="3">
+      <c r="A51" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" s="5">
         <v>30500000</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="C51" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="D51" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E51" s="3" t="s">
+      <c r="E51" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F51" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="F51" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G51" s="3" t="s">
+      <c r="G51" s="5" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A52" s="5">
+      <c r="A52" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B52" s="5">
         <v>30510000</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="C52" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="D52" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E52" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F52" s="5" t="s">
         <v>389</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A53" s="5">
+      <c r="A53" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" s="5">
         <v>30520000</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="C53" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="D53" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="E53" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E53" s="5" t="s">
+      <c r="F53" s="5" t="s">
         <v>423</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A54" s="3">
+      <c r="A54" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="5">
         <v>30530000</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="C54" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="D54" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E54" s="3" t="s">
+      <c r="E54" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F54" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="F54" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="G54" s="3" t="s">
+      <c r="G54" s="5" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A55" s="3">
+      <c r="A55" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B55" s="5">
         <v>30540000</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="C55" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="D55" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F55" s="5" t="s">
         <v>409</v>
       </c>
-      <c r="F55" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G55" s="3" t="s">
+      <c r="G55" s="5" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A56" s="5">
+      <c r="A56" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B56" s="5">
         <v>30550000</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="C56" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="D56" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="D56" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E56" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F56" s="5" t="s">
         <v>413</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>106</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A57" s="3">
+      <c r="A57" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B57" s="5">
         <v>30560000</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="C57" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="D57" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F57" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="F57" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="G57" s="3" t="s">
+      <c r="G57" s="5" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A58" s="5">
+      <c r="A58" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" s="5">
         <v>30570000</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="C58" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="D58" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="D58" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E58" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F58" s="5" t="s">
         <v>346</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A59" s="3">
+      <c r="A59" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B59" s="5">
         <v>30580000</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="C59" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="D59" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="E59" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="F59" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="F59" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G59" s="3" t="s">
+      <c r="G59" s="5" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A60" s="5">
+      <c r="A60" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B60" s="5">
         <v>30585000</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="C60" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="D60" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E60" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F60" s="5" t="s">
         <v>346</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>114</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A61" s="5">
+      <c r="A61" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B61" s="5">
         <v>30590000</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="C61" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="D61" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="D61" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E61" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F61" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A62" s="3">
+      <c r="A62" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B62" s="5">
         <v>30600000</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="C62" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="D62" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F62" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="F62" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G62" s="3" t="s">
+      <c r="G62" s="5" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A63" s="5">
+      <c r="A63" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" s="5">
         <v>30610000</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="C63" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="D63" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="D63" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E63" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F63" s="5" t="s">
         <v>346</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A64" s="3">
+      <c r="A64" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B64" s="5">
         <v>30630000</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="C64" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="D64" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="E64" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="F64" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="F64" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="G64" s="3" t="s">
+      <c r="G64" s="5" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A65" s="5">
+      <c r="A65" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B65" s="5">
         <v>30640000</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="C65" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="D65" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="D65" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E65" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F65" s="5" t="s">
         <v>346</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A66" s="3">
+      <c r="A66" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B66" s="5">
         <v>30650000</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="C66" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="D66" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="E66" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="F66" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="F66" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="G66" s="3" t="s">
+      <c r="G66" s="5" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A67" s="5">
+      <c r="A67" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B67" s="5">
         <v>30660000</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="C67" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="D67" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="D67" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E67" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F67" s="5" t="s">
         <v>346</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>128</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A68" s="3">
+      <c r="A68" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B68" s="5">
         <v>30670000</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="C68" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="D68" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E68" s="3" t="s">
+      <c r="E68" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F68" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="F68" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G68" s="3" t="s">
+      <c r="G68" s="5" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A69" s="5">
+      <c r="A69" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B69" s="5">
         <v>30680000</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="C69" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="D69" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="D69" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E69" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F69" s="5" t="s">
         <v>389</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>132</v>
       </c>
       <c r="G69" s="5" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A70" s="3">
+      <c r="A70" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" s="5">
         <v>30690000</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="C70" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="D70" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E70" s="3" t="s">
+      <c r="E70" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F70" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="F70" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="G70" s="3" t="s">
+      <c r="G70" s="5" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A71" s="5">
+      <c r="A71" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B71" s="5">
         <v>30700000</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="C71" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="D71" s="5" t="s">
         <v>344</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="E71" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E71" s="5" t="s">
+      <c r="F71" s="5" t="s">
         <v>354</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>136</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A72" s="3">
+      <c r="A72" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B72" s="5">
         <v>30710000</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="C72" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="D72" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="D72" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E72" s="3" t="s">
+      <c r="E72" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F72" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="F72" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G72" s="3" t="s">
+      <c r="G72" s="5" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A73" s="5">
+      <c r="A73" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B73" s="5">
         <v>30720000</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="C73" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="D73" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="D73" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E73" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F73" s="5" t="s">
         <v>346</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A74" s="3">
+      <c r="A74" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B74" s="5">
         <v>30730000</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="C74" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="D74" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="D74" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E74" s="3" t="s">
+      <c r="E74" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F74" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="F74" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="G74" s="3" t="s">
+      <c r="G74" s="5" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A75" s="3">
+      <c r="A75" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B75" s="5">
         <v>30740000</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="C75" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="D75" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="D75" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E75" s="3" t="s">
+      <c r="E75" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F75" s="5" t="s">
         <v>414</v>
       </c>
-      <c r="F75" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="G75" s="3" t="s">
+      <c r="G75" s="5" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A76" s="5">
+      <c r="A76" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B76" s="5">
         <v>30750000</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="C76" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="D76" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="D76" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E76" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F76" s="5" t="s">
         <v>413</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>146</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A77" s="3">
+      <c r="A77" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B77" s="5">
         <v>30760000</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="C77" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="D77" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="D77" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E77" s="3" t="s">
+      <c r="E77" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F77" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="F77" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G77" s="3" t="s">
+      <c r="G77" s="5" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A78" s="5">
+      <c r="A78" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B78" s="5">
         <v>30770000</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="C78" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="D78" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="D78" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E78" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F78" s="5" t="s">
         <v>413</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A79" s="3">
+      <c r="A79" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B79" s="5">
         <v>30780000</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="C79" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="D79" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="D79" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E79" s="3" t="s">
+      <c r="E79" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F79" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="F79" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="G79" s="3" t="s">
+      <c r="G79" s="5" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A80" s="5">
+      <c r="A80" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B80" s="5">
         <v>30800000</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="C80" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="D80" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="D80" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E80" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F80" s="5" t="s">
         <v>415</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A81" s="3">
+      <c r="A81" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B81" s="5">
         <v>30810000</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="C81" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="D81" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="D81" s="3" t="s">
+      <c r="E81" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E81" s="3" t="s">
+      <c r="F81" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="F81" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="G81" s="3" t="s">
+      <c r="G81" s="5" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A82" s="5">
+      <c r="A82" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B82" s="5">
         <v>30820000</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="C82" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C82" s="5" t="s">
+      <c r="D82" s="5" t="s">
         <v>432</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="E82" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E82" s="5" t="s">
+      <c r="F82" s="5" t="s">
         <v>424</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>158</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A83" s="3">
+      <c r="A83" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B83" s="5">
         <v>30830000</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="C83" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="D83" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="E83" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E83" s="3" t="s">
+      <c r="F83" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="F83" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="G83" s="3" t="s">
+      <c r="G83" s="5" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A84" s="5">
+      <c r="A84" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B84" s="5">
         <v>30840000</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="C84" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C84" s="5" t="s">
+      <c r="D84" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="E84" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E84" s="5" t="s">
+      <c r="F84" s="5" t="s">
         <v>423</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>162</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A85" s="5">
+      <c r="A85" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B85" s="5">
         <v>30850000</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="C85" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="D85" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="E85" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E85" s="5" t="s">
+      <c r="F85" s="5" t="s">
         <v>419</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>164</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A86" s="3">
+      <c r="A86" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B86" s="5">
         <v>30860000</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="C86" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="D86" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="D86" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E86" s="3" t="s">
+      <c r="E86" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F86" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="F86" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="G86" s="3" t="s">
+      <c r="G86" s="5" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A87" s="5">
+      <c r="A87" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B87" s="5">
         <v>30870000</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="C87" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="C87" s="5" t="s">
+      <c r="D87" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="E87" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E87" s="5" t="s">
+      <c r="F87" s="5" t="s">
         <v>358</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>168</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A88" s="3">
+      <c r="A88" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B88" s="5">
         <v>30880000</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="C88" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="D88" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="D88" s="3" t="s">
+      <c r="E88" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E88" s="3" t="s">
+      <c r="F88" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="F88" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="G88" s="3" t="s">
+      <c r="G88" s="5" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A89" s="5">
+      <c r="A89" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B89" s="5">
         <v>30890000</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="C89" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C89" s="5" t="s">
+      <c r="D89" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="E89" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E89" s="5" t="s">
+      <c r="F89" s="5" t="s">
         <v>358</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>172</v>
       </c>
       <c r="G89" s="5" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A90" s="3">
+      <c r="A90" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B90" s="5">
         <v>30900000</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="C90" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="D90" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="D90" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E90" s="3" t="s">
+      <c r="E90" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="F90" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="G90" s="3" t="s">
+      <c r="G90" s="5" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A91" s="3">
+      <c r="A91" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B91" s="5">
         <v>30910000</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="C91" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="D91" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="D91" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E91" s="3" t="s">
+      <c r="E91" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F91" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="F91" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="G91" s="3" t="s">
+      <c r="G91" s="5" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A92" s="5">
+      <c r="A92" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B92" s="5">
         <v>30920000</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="C92" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="C92" s="5" t="s">
+      <c r="D92" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="D92" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E92" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F92" s="5" t="s">
         <v>361</v>
-      </c>
-      <c r="F92" s="5" t="s">
-        <v>178</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A93" s="3">
+      <c r="A93" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B93" s="5">
         <v>30930000</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="C93" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="D93" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="D93" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E93" s="3" t="s">
+      <c r="E93" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F93" s="5" t="s">
         <v>414</v>
       </c>
-      <c r="F93" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="G93" s="3" t="s">
+      <c r="G93" s="5" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A94" s="5">
+      <c r="A94" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B94" s="5">
         <v>30940000</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="C94" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C94" s="5" t="s">
+      <c r="D94" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="D94" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E94" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F94" s="5" t="s">
         <v>408</v>
-      </c>
-      <c r="F94" s="5" t="s">
-        <v>182</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A95" s="3">
+      <c r="A95" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B95" s="5">
         <v>30950000</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="C95" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="D95" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="D95" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E95" s="3" t="s">
+      <c r="E95" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F95" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="F95" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="G95" s="3" t="s">
+      <c r="G95" s="5" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A96" s="5">
+      <c r="A96" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B96" s="5">
         <v>30960000</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="C96" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="C96" s="5" t="s">
+      <c r="D96" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="E96" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E96" s="5" t="s">
+      <c r="F96" s="5" t="s">
         <v>365</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>186</v>
       </c>
       <c r="G96" s="5" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A97" s="5">
+      <c r="A97" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B97" s="5">
         <v>30970000</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="C97" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="C97" s="5" t="s">
+      <c r="D97" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="D97" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E97" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F97" s="5" t="s">
         <v>409</v>
-      </c>
-      <c r="F97" s="5" t="s">
-        <v>188</v>
       </c>
       <c r="G97" s="5" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A98" s="3">
+      <c r="A98" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B98" s="5">
         <v>30980000</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="C98" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="D98" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="D98" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E98" s="3" t="s">
+      <c r="E98" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F98" s="5" t="s">
         <v>409</v>
       </c>
-      <c r="F98" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="G98" s="3" t="s">
+      <c r="G98" s="5" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A99" s="3">
+      <c r="A99" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B99" s="5">
         <v>30990000</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="C99" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="C99" s="3" t="s">
+      <c r="D99" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="D99" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E99" s="3" t="s">
+      <c r="E99" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F99" s="5" t="s">
         <v>409</v>
       </c>
-      <c r="F99" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="G99" s="3" t="s">
+      <c r="G99" s="5" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A100" s="5">
+      <c r="A100" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B100" s="5">
         <v>31000000</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="C100" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C100" s="5" t="s">
+      <c r="D100" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="D100" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E100" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F100" s="5" t="s">
         <v>414</v>
-      </c>
-      <c r="F100" s="5" t="s">
-        <v>194</v>
       </c>
       <c r="G100" s="5" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A101" s="5">
+      <c r="A101" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B101" s="5">
         <v>31010000</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="C101" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="C101" s="5" t="s">
+      <c r="D101" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="E101" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E101" s="5" t="s">
+      <c r="F101" s="5" t="s">
         <v>411</v>
-      </c>
-      <c r="F101" s="5" t="s">
-        <v>196</v>
       </c>
       <c r="G101" s="5" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A102" s="3">
+      <c r="A102" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="B102" s="5">
         <v>31020000</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="C102" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="C102" s="3" t="s">
+      <c r="D102" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="D102" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E102" s="3" t="s">
+      <c r="E102" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F102" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="F102" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="G102" s="3" t="s">
+      <c r="G102" s="5" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A103" s="5">
+      <c r="A103" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B103" s="5">
         <v>31030000</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="C103" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C103" s="5" t="s">
+      <c r="D103" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="D103" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E103" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F103" s="5" t="s">
         <v>415</v>
-      </c>
-      <c r="F103" s="5" t="s">
-        <v>199</v>
       </c>
       <c r="G103" s="5" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A104" s="3">
+      <c r="A104" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B104" s="5">
         <v>31040000</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="C104" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C104" s="3" t="s">
+      <c r="D104" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="D104" s="3" t="s">
+      <c r="E104" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E104" s="3" t="s">
+      <c r="F104" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="F104" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="G104" s="3" t="s">
+      <c r="G104" s="5" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A105" s="3">
+      <c r="A105" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B105" s="5">
         <v>31050000</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="C105" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C105" s="3" t="s">
+      <c r="D105" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="D105" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E105" s="3" t="s">
+      <c r="E105" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F105" s="5" t="s">
         <v>414</v>
       </c>
-      <c r="F105" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="G105" s="3" t="s">
+      <c r="G105" s="5" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A106" s="5">
+      <c r="A106" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B106" s="5">
         <v>31060000</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="C106" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="C106" s="5" t="s">
+      <c r="D106" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="D106" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E106" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F106" s="5" t="s">
         <v>370</v>
-      </c>
-      <c r="F106" s="5" t="s">
-        <v>205</v>
       </c>
       <c r="G106" s="5" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A107" s="3">
+      <c r="A107" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B107" s="5">
         <v>31070000</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="C107" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="D107" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="D107" s="3" t="s">
+      <c r="E107" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E107" s="3" t="s">
+      <c r="F107" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="F107" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="G107" s="3" t="s">
+      <c r="G107" s="5" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A108" s="5">
+      <c r="A108" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B108" s="5">
         <v>31080000</v>
       </c>
-      <c r="B108" s="5" t="s">
+      <c r="C108" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C108" s="5" t="s">
+      <c r="D108" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="D108" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E108" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F108" s="5" t="s">
         <v>389</v>
-      </c>
-      <c r="F108" s="5" t="s">
-        <v>209</v>
       </c>
       <c r="G108" s="5" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A109" s="3">
+      <c r="A109" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B109" s="5">
         <v>31090000</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="C109" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C109" s="3" t="s">
+      <c r="D109" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="D109" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E109" s="3" t="s">
+      <c r="E109" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F109" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="F109" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G109" s="3" t="s">
+      <c r="G109" s="5" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A110" s="5">
+      <c r="A110" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B110" s="5">
         <v>31100000</v>
       </c>
-      <c r="B110" s="5" t="s">
+      <c r="C110" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="C110" s="5" t="s">
+      <c r="D110" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="D110" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E110" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F110" s="5" t="s">
         <v>415</v>
-      </c>
-      <c r="F110" s="5" t="s">
-        <v>213</v>
       </c>
       <c r="G110" s="5" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A111" s="5">
+      <c r="A111" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B111" s="5">
         <v>31110000</v>
       </c>
-      <c r="B111" s="5" t="s">
+      <c r="C111" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C111" s="5" t="s">
+      <c r="D111" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="D111" s="5" t="s">
+      <c r="E111" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E111" s="5" t="s">
+      <c r="F111" s="5" t="s">
         <v>365</v>
-      </c>
-      <c r="F111" s="5" t="s">
-        <v>215</v>
       </c>
       <c r="G111" s="5" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A112" s="3">
+      <c r="A112" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B112" s="5">
         <v>31120000</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="C112" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C112" s="3" t="s">
+      <c r="D112" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="D112" s="3" t="s">
+      <c r="E112" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E112" s="3" t="s">
+      <c r="F112" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="F112" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="G112" s="3" t="s">
+      <c r="G112" s="5" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A113" s="5">
+      <c r="A113" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B113" s="5">
         <v>31130000</v>
       </c>
-      <c r="B113" s="5" t="s">
+      <c r="C113" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C113" s="5" t="s">
+      <c r="D113" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D113" s="5" t="s">
+      <c r="E113" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E113" s="5" t="s">
+      <c r="F113" s="5" t="s">
         <v>411</v>
-      </c>
-      <c r="F113" s="5" t="s">
-        <v>219</v>
       </c>
       <c r="G113" s="5" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A114" s="3">
+      <c r="A114" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B114" s="5">
         <v>31140000</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="C114" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="D114" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D114" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E114" s="3" t="s">
+      <c r="E114" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F114" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="F114" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="G114" s="3" t="s">
+      <c r="G114" s="5" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A115" s="5">
+      <c r="A115" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B115" s="5">
         <v>31150000</v>
       </c>
-      <c r="B115" s="5" t="s">
+      <c r="C115" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="C115" s="5" t="s">
+      <c r="D115" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="D115" s="5" t="s">
+      <c r="E115" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E115" s="5" t="s">
+      <c r="F115" s="5" t="s">
         <v>378</v>
-      </c>
-      <c r="F115" s="5" t="s">
-        <v>223</v>
       </c>
       <c r="G115" s="5" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A116" s="3">
+      <c r="A116" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B116" s="5">
         <v>31160000</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="C116" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="D116" s="5" t="s">
         <v>379</v>
       </c>
-      <c r="D116" s="3" t="s">
+      <c r="E116" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E116" s="3" t="s">
+      <c r="F116" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="F116" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="G116" s="3" t="s">
+      <c r="G116" s="5" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A117" s="5">
+      <c r="A117" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B117" s="5">
         <v>31170000</v>
       </c>
-      <c r="B117" s="5" t="s">
+      <c r="C117" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="C117" s="5" t="s">
+      <c r="D117" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="D117" s="5" t="s">
+      <c r="E117" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E117" s="5" t="s">
+      <c r="F117" s="5" t="s">
         <v>354</v>
-      </c>
-      <c r="F117" s="5" t="s">
-        <v>227</v>
       </c>
       <c r="G117" s="5" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A118" s="3">
+      <c r="A118" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B118" s="5">
         <v>31180000</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="C118" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="D118" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="D118" s="3" t="s">
+      <c r="E118" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E118" s="3" t="s">
+      <c r="F118" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="F118" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G118" s="3" t="s">
+      <c r="G118" s="5" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A119" s="5">
+      <c r="A119" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B119" s="5">
         <v>31190000</v>
       </c>
-      <c r="B119" s="5" t="s">
+      <c r="C119" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="C119" s="5" t="s">
+      <c r="D119" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="D119" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E119" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F119" s="5" t="s">
         <v>418</v>
-      </c>
-      <c r="F119" s="5" t="s">
-        <v>231</v>
       </c>
       <c r="G119" s="5" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A120" s="3">
+      <c r="A120" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B120" s="5">
         <v>31200000</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="C120" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="C120" s="3" t="s">
+      <c r="D120" s="5" t="s">
         <v>383</v>
       </c>
-      <c r="D120" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E120" s="3" t="s">
+      <c r="E120" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F120" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="F120" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="G120" s="3" t="s">
+      <c r="G120" s="5" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A121" s="5">
+      <c r="A121" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B121" s="5">
         <v>31210000</v>
       </c>
-      <c r="B121" s="5" t="s">
+      <c r="C121" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="C121" s="5" t="s">
+      <c r="D121" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="D121" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E121" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F121" s="5" t="s">
         <v>418</v>
-      </c>
-      <c r="F121" s="5" t="s">
-        <v>235</v>
       </c>
       <c r="G121" s="5" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A122" s="3">
+      <c r="A122" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B122" s="5">
         <v>31220000</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="C122" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="C122" s="3" t="s">
+      <c r="D122" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="D122" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E122" s="3" t="s">
+      <c r="E122" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F122" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="F122" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="G122" s="3" t="s">
+      <c r="G122" s="5" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A123" s="5">
+      <c r="A123" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B123" s="5">
         <v>31230000</v>
       </c>
-      <c r="B123" s="5" t="s">
+      <c r="C123" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="C123" s="5" t="s">
+      <c r="D123" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="D123" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E123" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F123" s="5" t="s">
         <v>413</v>
-      </c>
-      <c r="F123" s="5" t="s">
-        <v>239</v>
       </c>
       <c r="G123" s="5" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A124" s="3">
+      <c r="A124" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B124" s="5">
         <v>31240000</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="C124" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="C124" s="3" t="s">
+      <c r="D124" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="D124" s="3" t="s">
+      <c r="E124" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="E124" s="3" t="s">
+      <c r="F124" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="F124" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="G124" s="3" t="s">
+      <c r="G124" s="5" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A125" s="5">
+      <c r="A125" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B125" s="5">
         <v>31250000</v>
       </c>
-      <c r="B125" s="5" t="s">
+      <c r="C125" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="C125" s="5" t="s">
+      <c r="D125" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="D125" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E125" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F125" s="5" t="s">
         <v>346</v>
-      </c>
-      <c r="F125" s="5" t="s">
-        <v>243</v>
       </c>
       <c r="G125" s="5" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A126" s="3">
+      <c r="A126" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B126" s="5">
         <v>31260000</v>
       </c>
-      <c r="B126" s="3" t="s">
+      <c r="C126" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="C126" s="3" t="s">
+      <c r="D126" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D126" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E126" s="3" t="s">
+      <c r="E126" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F126" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="F126" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="G126" s="3" t="s">
+      <c r="G126" s="5" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A127" s="5">
+      <c r="A127" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B127" s="5">
         <v>31270000</v>
       </c>
-      <c r="B127" s="5" t="s">
+      <c r="C127" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="C127" s="5" t="s">
+      <c r="D127" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="D127" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E127" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F127" s="5" t="s">
         <v>415</v>
-      </c>
-      <c r="F127" s="5" t="s">
-        <v>247</v>
       </c>
       <c r="G127" s="5" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A128" s="12">
+      <c r="A128" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B128" s="10">
         <v>31280000</v>
       </c>
-      <c r="B128" s="12" t="s">
+      <c r="C128" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="C128" s="12" t="s">
+      <c r="D128" s="10" t="s">
         <v>391</v>
       </c>
-      <c r="D128" s="12" t="s">
-        <v>407</v>
-      </c>
-      <c r="E128" s="12" t="s">
+      <c r="E128" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="F128" s="10" t="s">
         <v>414</v>
       </c>
-      <c r="F128" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="G128" s="12" t="s">
+      <c r="G128" s="5" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A129" s="10">
+      <c r="A129" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B129" s="10">
         <v>31290000</v>
       </c>
-      <c r="B129" s="10" t="s">
+      <c r="C129" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="C129" s="10" t="s">
+      <c r="D129" s="10" t="s">
         <v>392</v>
       </c>
-      <c r="D129" s="10" t="s">
-        <v>407</v>
-      </c>
       <c r="E129" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="F129" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="F129" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="G129" s="10" t="s">
+      <c r="G129" s="5" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A130" s="12">
+      <c r="A130" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B130" s="10">
         <v>31300000</v>
       </c>
-      <c r="B130" s="12" t="s">
+      <c r="C130" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="C130" s="12" t="s">
+      <c r="D130" s="10" t="s">
         <v>393</v>
       </c>
-      <c r="D130" s="12" t="s">
-        <v>407</v>
-      </c>
-      <c r="E130" s="12" t="s">
+      <c r="E130" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="F130" s="10" t="s">
         <v>346</v>
       </c>
-      <c r="F130" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="G130" s="12" t="s">
+      <c r="G130" s="5" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A131" s="10">
+      <c r="A131" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B131" s="10">
         <v>31310000</v>
       </c>
-      <c r="B131" s="10" t="s">
+      <c r="C131" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C131" s="10" t="s">
+      <c r="D131" s="10" t="s">
         <v>394</v>
       </c>
-      <c r="D131" s="10" t="s">
+      <c r="E131" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="E131" s="10" t="s">
+      <c r="F131" s="10" t="s">
         <v>394</v>
       </c>
-      <c r="F131" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="G131" s="10" t="s">
+      <c r="G131" s="5" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A132" s="12">
+      <c r="A132" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B132" s="10">
         <v>31320000</v>
       </c>
-      <c r="B132" s="12" t="s">
+      <c r="C132" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="C132" s="12" t="s">
+      <c r="D132" s="10" t="s">
         <v>395</v>
       </c>
-      <c r="D132" s="12" t="s">
-        <v>407</v>
-      </c>
-      <c r="E132" s="12" t="s">
+      <c r="E132" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="F132" s="10" t="s">
         <v>346</v>
       </c>
-      <c r="F132" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="G132" s="12" t="s">
+      <c r="G132" s="5" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A133" s="10">
+      <c r="A133" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B133" s="10">
         <v>31330000</v>
       </c>
-      <c r="B133" s="10" t="s">
+      <c r="C133" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="C133" s="10" t="s">
+      <c r="D133" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="D133" s="10" t="s">
+      <c r="E133" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="E133" s="10" t="s">
+      <c r="F133" s="10" t="s">
         <v>412</v>
       </c>
-      <c r="F133" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="G133" s="10" t="s">
+      <c r="G133" s="5" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A134" s="12">
+      <c r="A134" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B134" s="10">
         <v>31340000</v>
       </c>
-      <c r="B134" s="12" t="s">
+      <c r="C134" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="C134" s="12" t="s">
+      <c r="D134" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="D134" s="12" t="s">
+      <c r="E134" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="E134" s="12" t="s">
+      <c r="F134" s="10" t="s">
         <v>412</v>
       </c>
-      <c r="F134" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="G134" s="12" t="s">
+      <c r="G134" s="5" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.8">
-      <c r="A135" s="10">
+      <c r="A135" s="10" t="s">
+        <v>552</v>
+      </c>
+      <c r="B135" s="10">
         <v>31350000</v>
       </c>
-      <c r="B135" s="10" t="s">
+      <c r="C135" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="C135" s="10" t="s">
+      <c r="D135" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="D135" s="10" t="s">
-        <v>407</v>
-      </c>
       <c r="E135" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="F135" s="10" t="s">
         <v>266</v>
-      </c>
-      <c r="F135" s="10" t="s">
-        <v>261</v>
       </c>
       <c r="G135" s="10" t="s">
         <v>266</v>
@@ -19987,8 +20065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13708FBC-0B91-46E5-AEFC-942007A5A68A}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A23" zoomScale="59" workbookViewId="0">
+      <selection activeCell="B38" sqref="A38:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.1" x14ac:dyDescent="0.8"/>

</xml_diff>